<commit_message>
Add player rank functionality
Add player rank functionality
</commit_message>
<xml_diff>
--- a/server/venv/Data/Data_Book.xlsx
+++ b/server/venv/Data/Data_Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nateb\Web\Draft-Project\server\venv\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FE1833-0096-4C8B-AC7B-507F41C3DFB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8903B8D6-E3A0-4E14-A2E6-123775D7747F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1512" yWindow="1092" windowWidth="21624" windowHeight="11244" xr2:uid="{8D78606D-69D0-4E31-9751-BBA7FEFEFD21}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>CeeDee Lamb</t>
   </si>
@@ -171,6 +171,15 @@
   </si>
   <si>
     <t>Josh Allen</t>
+  </si>
+  <si>
+    <t>Ja'Marr Chase</t>
+  </si>
+  <si>
+    <t>6'0"</t>
+  </si>
+  <si>
+    <t>CIN</t>
   </si>
 </sst>
 </file>
@@ -557,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4B74CF1-4E6F-4FE0-ACBC-3E6164382A77}">
-  <dimension ref="A1:AC5"/>
+  <dimension ref="A1:AC6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -989,6 +998,89 @@
         <v>17</v>
       </c>
     </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>262.72000000000003</v>
+      </c>
+      <c r="E6">
+        <v>23.72</v>
+      </c>
+      <c r="F6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6">
+        <v>24</v>
+      </c>
+      <c r="I6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6">
+        <v>201</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N6">
+        <v>3.1</v>
+      </c>
+      <c r="O6">
+        <v>14.1</v>
+      </c>
+      <c r="P6">
+        <v>7.3</v>
+      </c>
+      <c r="Q6">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="R6">
+        <v>8</v>
+      </c>
+      <c r="S6">
+        <v>15.2</v>
+      </c>
+      <c r="T6">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="U6">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="V6">
+        <v>7.2</v>
+      </c>
+      <c r="W6">
+        <v>8.1</v>
+      </c>
+      <c r="X6">
+        <v>20.6</v>
+      </c>
+      <c r="Y6">
+        <v>2.9</v>
+      </c>
+      <c r="Z6">
+        <v>6.4</v>
+      </c>
+      <c r="AA6">
+        <v>-1</v>
+      </c>
+      <c r="AB6">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AC6">
+        <v>1.9</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update data and add avg ppr
</commit_message>
<xml_diff>
--- a/server/venv/Data/Data_Book.xlsx
+++ b/server/venv/Data/Data_Book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nateb\Web\Draft-Project\server\venv\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8903B8D6-E3A0-4E14-A2E6-123775D7747F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6FE4D6-5D7C-4601-99CC-DDD3A0D5D88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1512" yWindow="1092" windowWidth="21624" windowHeight="11244" xr2:uid="{8D78606D-69D0-4E31-9751-BBA7FEFEFD21}"/>
+    <workbookView xWindow="1416" yWindow="1716" windowWidth="21624" windowHeight="11244" xr2:uid="{8D78606D-69D0-4E31-9751-BBA7FEFEFD21}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="77">
   <si>
     <t>CeeDee Lamb</t>
   </si>
@@ -180,6 +180,93 @@
   </si>
   <si>
     <t>CIN</t>
+  </si>
+  <si>
+    <t>week18</t>
+  </si>
+  <si>
+    <t>Jalen Hurts</t>
+  </si>
+  <si>
+    <t>PHI</t>
+  </si>
+  <si>
+    <t>6'1"</t>
+  </si>
+  <si>
+    <t>Dak Prescott</t>
+  </si>
+  <si>
+    <t>Lamar Jackson</t>
+  </si>
+  <si>
+    <t>BAL</t>
+  </si>
+  <si>
+    <t>Amon-Ra St. Brown</t>
+  </si>
+  <si>
+    <t>DET</t>
+  </si>
+  <si>
+    <t>Jordan Love</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>6'4"</t>
+  </si>
+  <si>
+    <t>Puka Nacua</t>
+  </si>
+  <si>
+    <t>LAR</t>
+  </si>
+  <si>
+    <t>Brock Purdy</t>
+  </si>
+  <si>
+    <t>Breece Hall</t>
+  </si>
+  <si>
+    <t>NYJ</t>
+  </si>
+  <si>
+    <t>A.J. Brown</t>
+  </si>
+  <si>
+    <t>Jared Goff</t>
+  </si>
+  <si>
+    <t>DJ Moore</t>
+  </si>
+  <si>
+    <t>CHI</t>
+  </si>
+  <si>
+    <t>Mike Evans</t>
+  </si>
+  <si>
+    <t>TB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travis Etienne </t>
+  </si>
+  <si>
+    <t>JAX</t>
+  </si>
+  <si>
+    <t>Patrick Mahomes</t>
+  </si>
+  <si>
+    <t>KC</t>
+  </si>
+  <si>
+    <t>Keenan Allen</t>
+  </si>
+  <si>
+    <t>LAC</t>
   </si>
 </sst>
 </file>
@@ -566,15 +653,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4B74CF1-4E6F-4FE0-ACBC-3E6164382A77}">
-  <dimension ref="A1:AC6"/>
+  <dimension ref="A1:AD21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -662,8 +749,11 @@
       <c r="AC1" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="AD1" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -674,10 +764,10 @@
         <v>3</v>
       </c>
       <c r="D2">
-        <v>369.58</v>
+        <v>392.6</v>
       </c>
       <c r="E2">
-        <v>23.72</v>
+        <v>24.16</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -695,58 +785,61 @@
         <v>17</v>
       </c>
       <c r="M2">
-        <v>11</v>
+        <v>9.0399999999999991</v>
       </c>
       <c r="N2">
-        <v>13</v>
+        <v>23.66</v>
       </c>
       <c r="O2">
-        <v>14</v>
+        <v>21.32</v>
       </c>
       <c r="P2">
-        <v>12</v>
+        <v>36.5</v>
       </c>
       <c r="Q2">
-        <v>7</v>
+        <v>27.76</v>
       </c>
       <c r="R2">
-        <v>9</v>
+        <v>13.86</v>
       </c>
       <c r="S2">
-        <v>11</v>
+        <v>24.3</v>
       </c>
       <c r="T2">
-        <v>-1</v>
+        <v>29.06</v>
       </c>
       <c r="U2">
-        <v>4</v>
+        <v>24.72</v>
       </c>
       <c r="V2">
-        <v>1</v>
+        <v>14.28</v>
       </c>
       <c r="W2">
-        <v>5</v>
+        <v>22.5</v>
       </c>
       <c r="X2">
-        <v>1</v>
+        <v>39.659999999999997</v>
       </c>
       <c r="Y2">
-        <v>11</v>
+        <v>-1</v>
       </c>
       <c r="Z2">
-        <v>10</v>
+        <v>20.52</v>
       </c>
       <c r="AA2">
-        <v>8</v>
+        <v>16.16</v>
       </c>
       <c r="AB2">
-        <v>17</v>
+        <v>24.98</v>
       </c>
       <c r="AC2">
-        <v>1</v>
+        <v>21.16</v>
+      </c>
+      <c r="AD2">
+        <v>23.06</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -757,7 +850,7 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <v>367.5</v>
+        <v>403.2</v>
       </c>
       <c r="E3">
         <v>23.72</v>
@@ -778,58 +871,61 @@
         <v>88</v>
       </c>
       <c r="M3">
-        <v>1</v>
+        <v>11.7</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>25.3</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="P3">
-        <v>10</v>
+        <v>14.8</v>
       </c>
       <c r="Q3">
-        <v>27</v>
+        <v>8.9</v>
       </c>
       <c r="R3">
-        <v>10</v>
+        <v>18.7</v>
       </c>
       <c r="S3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="T3">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="U3">
-        <v>1</v>
+        <v>28.1</v>
       </c>
       <c r="V3">
-        <v>1</v>
+        <v>39.5</v>
       </c>
       <c r="W3">
-        <v>1</v>
+        <v>16.5</v>
       </c>
       <c r="X3">
-        <v>1</v>
+        <v>17.3</v>
       </c>
       <c r="Y3">
-        <v>1</v>
+        <v>32.6</v>
       </c>
       <c r="Z3">
-        <v>1</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="AA3">
-        <v>8</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="AB3">
-        <v>17</v>
+        <v>25.2</v>
       </c>
       <c r="AC3">
-        <v>1</v>
+        <v>40.200000000000003</v>
+      </c>
+      <c r="AD3">
+        <v>35.5</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -843,7 +939,7 @@
         <v>391.3</v>
       </c>
       <c r="E4">
-        <v>23.72</v>
+        <v>24.46</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
@@ -864,58 +960,61 @@
         <v>10</v>
       </c>
       <c r="M4">
-        <v>10</v>
+        <v>25.9</v>
       </c>
       <c r="N4">
-        <v>10</v>
+        <v>22.5</v>
       </c>
       <c r="O4">
-        <v>10</v>
+        <v>22.9</v>
       </c>
       <c r="P4">
-        <v>10</v>
+        <v>48.7</v>
       </c>
       <c r="Q4">
-        <v>10</v>
+        <v>13.8</v>
       </c>
       <c r="R4">
-        <v>-1</v>
+        <v>14.2</v>
       </c>
       <c r="S4">
-        <v>-1</v>
+        <v>22.6</v>
       </c>
       <c r="T4">
-        <v>10</v>
+        <v>29.8</v>
       </c>
       <c r="U4">
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="V4">
-        <v>10</v>
+        <v>20.2</v>
       </c>
       <c r="W4">
-        <v>10</v>
+        <v>21.3</v>
       </c>
       <c r="X4">
-        <v>10</v>
+        <v>30.9</v>
       </c>
       <c r="Y4">
-        <v>10</v>
+        <v>22.3</v>
       </c>
       <c r="Z4">
-        <v>10</v>
+        <v>16.3</v>
       </c>
       <c r="AA4">
-        <v>8</v>
+        <v>41.7</v>
       </c>
       <c r="AB4">
-        <v>10</v>
+        <v>25.1</v>
       </c>
       <c r="AC4">
-        <v>10</v>
+        <v>13.1</v>
+      </c>
+      <c r="AD4">
+        <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -929,7 +1028,7 @@
         <v>376.4</v>
       </c>
       <c r="E5">
-        <v>23.72</v>
+        <v>23.52</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -947,58 +1046,61 @@
         <v>29</v>
       </c>
       <c r="M5">
-        <v>1</v>
+        <v>44.5</v>
       </c>
       <c r="N5">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="O5">
-        <v>3</v>
+        <v>30.7</v>
       </c>
       <c r="P5">
-        <v>4</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="Q5">
-        <v>5</v>
+        <v>32.1</v>
       </c>
       <c r="R5">
-        <v>6</v>
+        <v>28.3</v>
       </c>
       <c r="S5">
-        <v>7</v>
+        <v>25.8</v>
       </c>
       <c r="T5">
-        <v>8</v>
+        <v>25.2</v>
       </c>
       <c r="U5">
-        <v>9</v>
+        <v>12.5</v>
       </c>
       <c r="V5">
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="W5">
-        <v>11</v>
+        <v>30.6</v>
       </c>
       <c r="X5">
-        <v>12</v>
+        <v>25.4</v>
       </c>
       <c r="Y5">
-        <v>13</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="Z5">
-        <v>14</v>
+        <v>10.1</v>
       </c>
       <c r="AA5">
-        <v>15</v>
+        <v>-1</v>
       </c>
       <c r="AB5">
-        <v>16</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="AC5">
-        <v>17</v>
+        <v>13.6</v>
+      </c>
+      <c r="AD5">
+        <v>21.2</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1012,7 +1114,7 @@
         <v>262.72000000000003</v>
       </c>
       <c r="E6">
-        <v>23.72</v>
+        <v>16.420000000000002</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
@@ -1030,55 +1132,1348 @@
         <v>1</v>
       </c>
       <c r="M6">
-        <v>4.0999999999999996</v>
+        <v>9.1</v>
       </c>
       <c r="N6">
-        <v>3.1</v>
+        <v>8.1</v>
       </c>
       <c r="O6">
+        <v>26.1</v>
+      </c>
+      <c r="P6">
+        <v>14.3</v>
+      </c>
+      <c r="Q6">
+        <v>52.2</v>
+      </c>
+      <c r="R6">
+        <v>14</v>
+      </c>
+      <c r="S6">
+        <v>-1</v>
+      </c>
+      <c r="T6">
+        <v>25.2</v>
+      </c>
+      <c r="U6">
+        <v>8.1</v>
+      </c>
+      <c r="V6">
+        <v>23.4</v>
+      </c>
+      <c r="W6">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="X6">
+        <v>12.1</v>
+      </c>
+      <c r="Y6">
+        <v>31.62</v>
+      </c>
+      <c r="Z6">
+        <v>5.9</v>
+      </c>
+      <c r="AA6">
+        <v>10.4</v>
+      </c>
+      <c r="AB6">
+        <v>-1</v>
+      </c>
+      <c r="AC6">
+        <v>7.1</v>
+      </c>
+      <c r="AD6">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>356.8</v>
+      </c>
+      <c r="E7">
+        <v>21.87</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7">
+        <v>223</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>12.5</v>
+      </c>
+      <c r="N7">
+        <v>25.22</v>
+      </c>
+      <c r="O7">
+        <v>19.88</v>
+      </c>
+      <c r="P7">
+        <v>24.16</v>
+      </c>
+      <c r="Q7">
+        <v>27.32</v>
+      </c>
+      <c r="R7">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="S7">
+        <v>23.26</v>
+      </c>
+      <c r="T7">
+        <v>27.36</v>
+      </c>
+      <c r="U7">
+        <v>25.88</v>
+      </c>
+      <c r="V7">
+        <v>-1</v>
+      </c>
+      <c r="W7">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="X7">
+        <v>34.5</v>
+      </c>
+      <c r="Y7">
+        <v>23.92</v>
+      </c>
+      <c r="Z7">
+        <v>8.8800000000000008</v>
+      </c>
+      <c r="AA7">
+        <v>21.92</v>
+      </c>
+      <c r="AB7">
+        <v>23.44</v>
+      </c>
+      <c r="AC7">
+        <v>19.18</v>
+      </c>
+      <c r="AD7">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>342.8</v>
+      </c>
+      <c r="E8">
+        <v>20.7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <v>30</v>
+      </c>
+      <c r="I8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8">
+        <v>238</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+      <c r="M8">
+        <v>6.32</v>
+      </c>
+      <c r="N8">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="O8">
+        <v>14.36</v>
+      </c>
+      <c r="P8">
+        <v>14.34</v>
+      </c>
+      <c r="Q8">
+        <v>4.32</v>
+      </c>
+      <c r="R8">
+        <v>24.88</v>
+      </c>
+      <c r="S8">
+        <v>-1</v>
+      </c>
+      <c r="T8">
+        <v>28.06</v>
+      </c>
+      <c r="U8">
+        <v>28.36</v>
+      </c>
+      <c r="V8">
+        <v>37.86</v>
+      </c>
+      <c r="W8">
+        <v>16.16</v>
+      </c>
+      <c r="X8">
+        <v>32.24</v>
+      </c>
+      <c r="Y8">
+        <v>28.26</v>
+      </c>
+      <c r="Z8">
+        <v>17.940000000000001</v>
+      </c>
+      <c r="AA8">
+        <v>6.06</v>
+      </c>
+      <c r="AB8">
+        <v>18.62</v>
+      </c>
+      <c r="AC8">
+        <v>20.3</v>
+      </c>
+      <c r="AD8">
+        <v>25.16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>331.2</v>
+      </c>
+      <c r="E9">
+        <v>21.14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9">
+        <v>27</v>
+      </c>
+      <c r="I9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9">
+        <v>215</v>
+      </c>
+      <c r="K9">
+        <v>8</v>
+      </c>
+      <c r="M9">
+        <v>6.56</v>
+      </c>
+      <c r="N9">
+        <v>22.88</v>
+      </c>
+      <c r="O9">
+        <v>28.18</v>
+      </c>
+      <c r="P9">
+        <v>28.14</v>
+      </c>
+      <c r="Q9">
+        <v>9.94</v>
+      </c>
+      <c r="R9">
+        <v>17.12</v>
+      </c>
+      <c r="S9">
+        <v>33.880000000000003</v>
+      </c>
+      <c r="T9">
+        <v>11.98</v>
+      </c>
+      <c r="U9">
+        <v>11.48</v>
+      </c>
+      <c r="V9">
+        <v>13.02</v>
+      </c>
+      <c r="W9">
+        <v>23.96</v>
+      </c>
+      <c r="X9">
+        <v>14.98</v>
+      </c>
+      <c r="Y9">
+        <v>-1</v>
+      </c>
+      <c r="Z9">
+        <v>31.64</v>
+      </c>
+      <c r="AA9">
+        <v>18.54</v>
+      </c>
+      <c r="AB9">
+        <v>22.58</v>
+      </c>
+      <c r="AC9">
+        <v>36.340000000000003</v>
+      </c>
+      <c r="AD9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>330.9</v>
+      </c>
+      <c r="E10">
+        <v>20.74</v>
+      </c>
+      <c r="F10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10">
+        <v>24</v>
+      </c>
+      <c r="I10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10">
+        <v>202</v>
+      </c>
+      <c r="K10">
+        <v>14</v>
+      </c>
+      <c r="M10">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="N10">
+        <v>14.2</v>
+      </c>
+      <c r="O10">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="P10">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="Q10">
+        <v>-1</v>
+      </c>
+      <c r="R10">
+        <v>30.4</v>
+      </c>
+      <c r="S10">
+        <v>23.2</v>
+      </c>
+      <c r="T10">
+        <v>16.8</v>
+      </c>
+      <c r="U10">
+        <v>-1</v>
+      </c>
+      <c r="V10">
+        <v>30.5</v>
+      </c>
+      <c r="W10">
+        <v>21.7</v>
+      </c>
+      <c r="X10">
+        <v>18.5</v>
+      </c>
+      <c r="Y10">
+        <v>12.9</v>
+      </c>
+      <c r="Z10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="AA10">
+        <v>24.2</v>
+      </c>
+      <c r="AB10">
+        <v>28.6</v>
+      </c>
+      <c r="AC10">
+        <v>22.1</v>
+      </c>
+      <c r="AD10">
+        <v>27.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>319.10000000000002</v>
+      </c>
+      <c r="E11">
+        <v>19.420000000000002</v>
+      </c>
+      <c r="F11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11">
+        <v>25</v>
+      </c>
+      <c r="I11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11">
+        <v>219</v>
+      </c>
+      <c r="K11">
+        <v>10</v>
+      </c>
+      <c r="M11">
+        <v>23</v>
+      </c>
+      <c r="N11">
+        <v>20.34</v>
+      </c>
+      <c r="O11">
+        <v>24.26</v>
+      </c>
+      <c r="P11">
+        <v>17.64</v>
+      </c>
+      <c r="Q11">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="R11">
+        <v>-1</v>
+      </c>
+      <c r="S11">
+        <v>15.3</v>
+      </c>
+      <c r="T11">
+        <v>14.56</v>
+      </c>
+      <c r="U11">
+        <v>13.82</v>
+      </c>
+      <c r="V11">
+        <v>16.66</v>
+      </c>
+      <c r="W11">
+        <v>20.88</v>
+      </c>
+      <c r="X11">
+        <v>26.62</v>
+      </c>
+      <c r="Y11">
+        <v>23.68</v>
+      </c>
+      <c r="Z11">
+        <v>8.92</v>
+      </c>
+      <c r="AA11">
+        <v>17.46</v>
+      </c>
+      <c r="AB11">
+        <v>23.96</v>
+      </c>
+      <c r="AC11">
+        <v>28.44</v>
+      </c>
+      <c r="AD11">
+        <v>18.54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>298.5</v>
+      </c>
+      <c r="E12">
+        <v>17.559999999999999</v>
+      </c>
+      <c r="F12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12">
+        <v>22</v>
+      </c>
+      <c r="I12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12">
+        <v>205</v>
+      </c>
+      <c r="K12">
+        <v>17</v>
+      </c>
+      <c r="M12">
+        <v>21.9</v>
+      </c>
+      <c r="N12">
+        <v>30.1</v>
+      </c>
+      <c r="O12">
+        <v>12.2</v>
+      </c>
+      <c r="P12">
+        <v>31.3</v>
+      </c>
+      <c r="Q12">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="R12">
+        <v>6.6</v>
+      </c>
+      <c r="S12">
+        <v>23.4</v>
+      </c>
+      <c r="T12">
+        <v>7.3</v>
+      </c>
+      <c r="U12">
+        <v>6.2</v>
+      </c>
+      <c r="V12">
+        <v>-1</v>
+      </c>
+      <c r="W12">
+        <v>18.7</v>
+      </c>
+      <c r="X12">
+        <v>6.7</v>
+      </c>
+      <c r="Y12">
+        <v>23.9</v>
+      </c>
+      <c r="Z12">
+        <v>14</v>
+      </c>
+      <c r="AA12">
+        <v>10.3</v>
+      </c>
+      <c r="AB12">
+        <v>33</v>
+      </c>
+      <c r="AC12">
+        <v>18.7</v>
+      </c>
+      <c r="AD12">
         <v>14.1</v>
       </c>
-      <c r="P6">
-        <v>7.3</v>
-      </c>
-      <c r="Q6">
-        <v>37.200000000000003</v>
-      </c>
-      <c r="R6">
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>295.60000000000002</v>
+      </c>
+      <c r="E13">
+        <v>18.04</v>
+      </c>
+      <c r="F13" t="s">
         <v>8</v>
       </c>
-      <c r="S6">
-        <v>15.2</v>
-      </c>
-      <c r="T6">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="U6">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="V6">
-        <v>7.2</v>
-      </c>
-      <c r="W6">
-        <v>8.1</v>
-      </c>
-      <c r="X6">
-        <v>20.6</v>
-      </c>
-      <c r="Y6">
-        <v>2.9</v>
-      </c>
-      <c r="Z6">
+      <c r="H13">
+        <v>24</v>
+      </c>
+      <c r="I13" t="s">
+        <v>51</v>
+      </c>
+      <c r="J13">
+        <v>220</v>
+      </c>
+      <c r="K13">
+        <v>13</v>
+      </c>
+      <c r="M13">
+        <v>16.8</v>
+      </c>
+      <c r="N13">
+        <v>14.74</v>
+      </c>
+      <c r="O13">
+        <v>20.3</v>
+      </c>
+      <c r="P13">
+        <v>21.32</v>
+      </c>
+      <c r="Q13">
+        <v>26.08</v>
+      </c>
+      <c r="R13">
+        <v>7.7</v>
+      </c>
+      <c r="S13">
+        <v>12.78</v>
+      </c>
+      <c r="T13">
+        <v>18.3</v>
+      </c>
+      <c r="U13">
+        <v>-1</v>
+      </c>
+      <c r="V13">
+        <v>23.84</v>
+      </c>
+      <c r="W13">
+        <v>26.72</v>
+      </c>
+      <c r="X13">
+        <v>10.46</v>
+      </c>
+      <c r="Y13">
+        <v>29.46</v>
+      </c>
+      <c r="Z13">
+        <v>21.42</v>
+      </c>
+      <c r="AA13">
+        <v>25.68</v>
+      </c>
+      <c r="AB13">
+        <v>2.4</v>
+      </c>
+      <c r="AC13">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="AD13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>290.5</v>
+      </c>
+      <c r="E14">
+        <v>17.09</v>
+      </c>
+      <c r="F14" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14">
+        <v>22</v>
+      </c>
+      <c r="I14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14">
+        <v>217</v>
+      </c>
+      <c r="K14">
+        <v>20</v>
+      </c>
+      <c r="M14">
+        <v>15.7</v>
+      </c>
+      <c r="N14">
+        <v>0.9</v>
+      </c>
+      <c r="O14">
+        <v>3.7</v>
+      </c>
+      <c r="P14">
+        <v>9.9</v>
+      </c>
+      <c r="Q14">
+        <v>28.4</v>
+      </c>
+      <c r="R14">
+        <v>20.3</v>
+      </c>
+      <c r="S14">
+        <v>-1</v>
+      </c>
+      <c r="T14">
+        <v>21.3</v>
+      </c>
+      <c r="U14">
+        <v>10</v>
+      </c>
+      <c r="V14">
+        <v>10.5</v>
+      </c>
+      <c r="W14">
+        <v>18.3</v>
+      </c>
+      <c r="X14">
+        <v>11.9</v>
+      </c>
+      <c r="Y14">
+        <v>10.5</v>
+      </c>
+      <c r="Z14">
+        <v>26.6</v>
+      </c>
+      <c r="AA14">
+        <v>2.8</v>
+      </c>
+      <c r="AB14">
+        <v>43.1</v>
+      </c>
+      <c r="AC14">
+        <v>27.6</v>
+      </c>
+      <c r="AD14">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>289.60000000000002</v>
+      </c>
+      <c r="E15">
+        <v>17.04</v>
+      </c>
+      <c r="F15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15">
+        <v>26</v>
+      </c>
+      <c r="I15" t="s">
+        <v>51</v>
+      </c>
+      <c r="J15">
+        <v>226</v>
+      </c>
+      <c r="K15">
+        <v>11</v>
+      </c>
+      <c r="M15">
+        <v>14.9</v>
+      </c>
+      <c r="N15">
+        <v>6.9</v>
+      </c>
+      <c r="O15">
+        <v>22.1</v>
+      </c>
+      <c r="P15">
+        <v>38.5</v>
+      </c>
+      <c r="Q15">
+        <v>18.7</v>
+      </c>
+      <c r="R15">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="S15">
+        <v>29.7</v>
+      </c>
+      <c r="T15">
+        <v>33</v>
+      </c>
+      <c r="U15">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="V15">
+        <v>-1</v>
+      </c>
+      <c r="W15">
+        <v>1.8</v>
+      </c>
+      <c r="X15">
+        <v>14.7</v>
+      </c>
+      <c r="Y15">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="Z15">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="AA15">
+        <v>10.6</v>
+      </c>
+      <c r="AB15">
+        <v>14</v>
+      </c>
+      <c r="AC15">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="AD15">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>289.10000000000002</v>
+      </c>
+      <c r="E16">
+        <v>17.71</v>
+      </c>
+      <c r="F16" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16">
+        <v>29</v>
+      </c>
+      <c r="I16" t="s">
+        <v>59</v>
+      </c>
+      <c r="J16">
+        <v>217</v>
+      </c>
+      <c r="K16">
+        <v>16</v>
+      </c>
+      <c r="M16">
+        <v>14.02</v>
+      </c>
+      <c r="N16">
+        <v>22.92</v>
+      </c>
+      <c r="O16">
+        <v>18.02</v>
+      </c>
+      <c r="P16">
+        <v>11.4</v>
+      </c>
+      <c r="Q16">
+        <v>27.44</v>
+      </c>
+      <c r="R16">
+        <v>22.42</v>
+      </c>
+      <c r="S16">
+        <v>9.36</v>
+      </c>
+      <c r="T16">
+        <v>12.68</v>
+      </c>
+      <c r="U16">
+        <v>-1</v>
+      </c>
+      <c r="V16">
+        <v>21.12</v>
+      </c>
+      <c r="W16">
+        <v>13.74</v>
+      </c>
+      <c r="X16">
+        <v>18.18</v>
+      </c>
+      <c r="Y16">
+        <v>16.32</v>
+      </c>
+      <c r="Z16">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="AA16">
+        <v>31.12</v>
+      </c>
+      <c r="AB16">
+        <v>14.28</v>
+      </c>
+      <c r="AC16">
+        <v>10.84</v>
+      </c>
+      <c r="AD16">
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>286.5</v>
+      </c>
+      <c r="E17">
+        <v>16.91</v>
+      </c>
+      <c r="F17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17">
+        <v>27</v>
+      </c>
+      <c r="I17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17">
+        <v>210</v>
+      </c>
+      <c r="K17">
+        <v>2</v>
+      </c>
+      <c r="M17">
+        <v>4.5</v>
+      </c>
+      <c r="N17">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="O17">
+        <v>13.1</v>
+      </c>
+      <c r="P17">
+        <v>27.1</v>
+      </c>
+      <c r="Q17">
+        <v>49</v>
+      </c>
+      <c r="R17">
+        <v>10.1</v>
+      </c>
+      <c r="S17">
+        <v>13.4</v>
+      </c>
+      <c r="T17">
+        <v>9.5</v>
+      </c>
+      <c r="U17">
+        <v>5.4</v>
+      </c>
+      <c r="V17">
+        <v>10.9</v>
+      </c>
+      <c r="W17">
+        <v>22.6</v>
+      </c>
+      <c r="X17">
+        <v>22.4</v>
+      </c>
+      <c r="Y17">
+        <v>-1</v>
+      </c>
+      <c r="Z17">
+        <v>26.8</v>
+      </c>
+      <c r="AA17">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="AB17">
+        <v>4.8</v>
+      </c>
+      <c r="AC17">
+        <v>30.9</v>
+      </c>
+      <c r="AD17">
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>282.5</v>
+      </c>
+      <c r="E18">
+        <v>16.62</v>
+      </c>
+      <c r="F18" t="s">
+        <v>70</v>
+      </c>
+      <c r="H18">
+        <v>30</v>
+      </c>
+      <c r="I18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18">
+        <v>231</v>
+      </c>
+      <c r="K18">
+        <v>13</v>
+      </c>
+      <c r="M18">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="N18">
+        <v>29.1</v>
+      </c>
+      <c r="O18">
+        <v>17</v>
+      </c>
+      <c r="P18">
+        <v>7</v>
+      </c>
+      <c r="Q18">
+        <v>-1</v>
+      </c>
+      <c r="R18">
+        <v>8.9</v>
+      </c>
+      <c r="S18">
+        <v>20.2</v>
+      </c>
+      <c r="T18">
+        <v>12.9</v>
+      </c>
+      <c r="U18">
+        <v>12.7</v>
+      </c>
+      <c r="V18">
+        <v>26.3</v>
+      </c>
+      <c r="W18">
+        <v>15.3</v>
+      </c>
+      <c r="X18">
+        <v>25</v>
+      </c>
+      <c r="Y18">
+        <v>29.2</v>
+      </c>
+      <c r="Z18">
+        <v>1.8</v>
+      </c>
+      <c r="AA18">
+        <v>15.7</v>
+      </c>
+      <c r="AB18">
+        <v>27.6</v>
+      </c>
+      <c r="AC18">
+        <v>10</v>
+      </c>
+      <c r="AD18">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>282.39999999999998</v>
+      </c>
+      <c r="E19">
+        <v>16.61</v>
+      </c>
+      <c r="F19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19">
+        <v>25</v>
+      </c>
+      <c r="I19" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19">
+        <v>215</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>21.4</v>
+      </c>
+      <c r="N19">
+        <v>6.2</v>
+      </c>
+      <c r="O19">
+        <v>17.8</v>
+      </c>
+      <c r="P19">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="Q19">
+        <v>36.4</v>
+      </c>
+      <c r="R19">
+        <v>23.3</v>
+      </c>
+      <c r="S19">
+        <v>22.7</v>
+      </c>
+      <c r="T19">
+        <v>25.9</v>
+      </c>
+      <c r="U19">
+        <v>-1</v>
+      </c>
+      <c r="V19">
         <v>6.4</v>
       </c>
-      <c r="AA6">
-        <v>-1</v>
-      </c>
-      <c r="AB6">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="AC6">
-        <v>1.9</v>
+      <c r="W19">
+        <v>8.9</v>
+      </c>
+      <c r="X19">
+        <v>12.6</v>
+      </c>
+      <c r="Y19">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="Z19">
+        <v>17.2</v>
+      </c>
+      <c r="AA19">
+        <v>9.9</v>
+      </c>
+      <c r="AB19">
+        <v>6.1</v>
+      </c>
+      <c r="AC19">
+        <v>25.8</v>
+      </c>
+      <c r="AD19">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>280.2</v>
+      </c>
+      <c r="E20">
+        <v>18.39</v>
+      </c>
+      <c r="F20" t="s">
+        <v>74</v>
+      </c>
+      <c r="H20">
+        <v>28</v>
+      </c>
+      <c r="I20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20">
+        <v>225</v>
+      </c>
+      <c r="K20">
+        <v>8</v>
+      </c>
+      <c r="M20">
+        <v>19.54</v>
+      </c>
+      <c r="N20">
+        <v>21.2</v>
+      </c>
+      <c r="O20">
+        <v>25.68</v>
+      </c>
+      <c r="P20">
+        <v>13.22</v>
+      </c>
+      <c r="Q20">
+        <v>19.239999999999998</v>
+      </c>
+      <c r="R20">
+        <v>17.34</v>
+      </c>
+      <c r="S20">
+        <v>33.86</v>
+      </c>
+      <c r="T20">
+        <v>5.6</v>
+      </c>
+      <c r="U20">
+        <v>15.8</v>
+      </c>
+      <c r="V20">
+        <v>-1</v>
+      </c>
+      <c r="W20">
+        <v>16.88</v>
+      </c>
+      <c r="X20">
+        <v>20.82</v>
+      </c>
+      <c r="Y20">
+        <v>13</v>
+      </c>
+      <c r="Z20">
+        <v>13.64</v>
+      </c>
+      <c r="AA20">
+        <v>15.7</v>
+      </c>
+      <c r="AB20">
+        <v>16.7</v>
+      </c>
+      <c r="AC20">
+        <v>12</v>
+      </c>
+      <c r="AD20">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>278.89999999999998</v>
+      </c>
+      <c r="E21">
+        <v>21.45</v>
+      </c>
+      <c r="F21" t="s">
+        <v>76</v>
+      </c>
+      <c r="H21">
+        <v>32</v>
+      </c>
+      <c r="I21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21">
+        <v>211</v>
+      </c>
+      <c r="K21">
+        <v>13</v>
+      </c>
+      <c r="M21">
+        <v>14.2</v>
+      </c>
+      <c r="N21">
+        <v>31.1</v>
+      </c>
+      <c r="O21">
+        <v>45.46</v>
+      </c>
+      <c r="P21">
+        <v>12.2</v>
+      </c>
+      <c r="Q21">
+        <v>-1</v>
+      </c>
+      <c r="R21">
+        <v>21.5</v>
+      </c>
+      <c r="S21">
+        <v>9.5</v>
+      </c>
+      <c r="T21">
+        <v>14.9</v>
+      </c>
+      <c r="U21">
+        <v>15.7</v>
+      </c>
+      <c r="V21">
+        <v>40.5</v>
+      </c>
+      <c r="W21">
+        <v>27.6</v>
+      </c>
+      <c r="X21">
+        <v>22.6</v>
+      </c>
+      <c r="Y21">
+        <v>10.8</v>
+      </c>
+      <c r="Z21">
+        <v>12.8</v>
+      </c>
+      <c r="AA21">
+        <v>-1</v>
+      </c>
+      <c r="AB21">
+        <v>-1</v>
+      </c>
+      <c r="AC21">
+        <v>-1</v>
+      </c>
+      <c r="AD21">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>